<commit_message>
Scatter Plots & Basic ML-Model
</commit_message>
<xml_diff>
--- a/Data/summary_after_quality_preprocessing.xlsx
+++ b/Data/summary_after_quality_preprocessing.xlsx
@@ -455,52 +455,52 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="C2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="D2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="E2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="F2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="G2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="H2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="I2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="J2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="K2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="L2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="M2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="N2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="O2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="P2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
       <c r="Q2" t="n">
-        <v>418727</v>
+        <v>48587</v>
       </c>
     </row>
     <row r="3">
@@ -510,52 +510,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16025.87056055616</v>
+        <v>18482.26115607056</v>
       </c>
       <c r="C3" t="n">
-        <v>22.19721919054659</v>
+        <v>2.945664478152592</v>
       </c>
       <c r="D3" t="n">
-        <v>44.24370771409534</v>
+        <v>43.23594788729496</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06995727526526831</v>
+        <v>0.07080083149813736</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5901267412896708</v>
+        <v>0.3693580587399922</v>
       </c>
       <c r="G3" t="n">
-        <v>136684.8155003141</v>
+        <v>130943.1803568856</v>
       </c>
       <c r="H3" t="n">
-        <v>60.05222944782639</v>
+        <v>67.66391483318583</v>
       </c>
       <c r="I3" t="n">
-        <v>3.35930645026473</v>
+        <v>3.217689361351802</v>
       </c>
       <c r="J3" t="n">
-        <v>2575.810833717435</v>
+        <v>2507.886269372466</v>
       </c>
       <c r="K3" t="n">
-        <v>882.0535400869779</v>
+        <v>913.8347380986684</v>
       </c>
       <c r="L3" t="n">
-        <v>470.4010055000035</v>
+        <v>462.4929754872703</v>
       </c>
       <c r="M3" t="n">
-        <v>1080.084900687083</v>
+        <v>1157.553899602774</v>
       </c>
       <c r="N3" t="n">
-        <v>1654.370677386459</v>
+        <v>1631.480181941672</v>
       </c>
       <c r="O3" t="n">
-        <v>171.2021242843244</v>
+        <v>198.3287240922613</v>
       </c>
       <c r="P3" t="n">
-        <v>7.961559481475997</v>
+        <v>6.949048243357278</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.449065859139726</v>
+        <v>6.450532035318089</v>
       </c>
     </row>
     <row r="4">
@@ -565,52 +565,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>22725.31225212247</v>
+        <v>28191.71108331252</v>
       </c>
       <c r="C4" t="n">
-        <v>12.79050270507313</v>
+        <v>1.411945396998974</v>
       </c>
       <c r="D4" t="n">
-        <v>30.50854345205629</v>
+        <v>29.69981647724367</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2550753031686338</v>
+        <v>0.2564944985987722</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6668924160647512</v>
+        <v>0.4826359678043436</v>
       </c>
       <c r="G4" t="n">
-        <v>61010.36764059852</v>
+        <v>75208.80070856874</v>
       </c>
       <c r="H4" t="n">
-        <v>18.45527609963105</v>
+        <v>14.93884860387811</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4583901067968621</v>
+        <v>0.4233053916825096</v>
       </c>
       <c r="J4" t="n">
-        <v>6056.727745373791</v>
+        <v>5739.409853448393</v>
       </c>
       <c r="K4" t="n">
-        <v>5085.673098268658</v>
+        <v>5662.93151213163</v>
       </c>
       <c r="L4" t="n">
-        <v>5543.813078125964</v>
+        <v>5213.825652896686</v>
       </c>
       <c r="M4" t="n">
-        <v>3901.557337587457</v>
+        <v>3860.971557146052</v>
       </c>
       <c r="N4" t="n">
-        <v>4207.203564328611</v>
+        <v>3466.857487148857</v>
       </c>
       <c r="O4" t="n">
-        <v>39.15883234356029</v>
+        <v>36.14278185225009</v>
       </c>
       <c r="P4" t="n">
-        <v>1.864314356717593</v>
+        <v>1.03435187816563</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.24622227768341</v>
+        <v>3.250982181878554</v>
       </c>
     </row>
     <row r="5">
@@ -638,10 +638,10 @@
         <v>34875</v>
       </c>
       <c r="H5" t="n">
-        <v>-2.06</v>
+        <v>28.84</v>
       </c>
       <c r="I5" t="n">
-        <v>2.472</v>
+        <v>2.514</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2116.195</v>
+        <v>2207.065</v>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -690,13 +690,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>93638</v>
+        <v>37392</v>
       </c>
       <c r="H6" t="n">
-        <v>46.66</v>
+        <v>56.36</v>
       </c>
       <c r="I6" t="n">
-        <v>2.931</v>
+        <v>2.759</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -714,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>132.0226667</v>
+        <v>210.8967606</v>
       </c>
       <c r="P6" t="n">
-        <v>6.891</v>
+        <v>6.489</v>
       </c>
       <c r="Q6" t="n">
         <v>4</v>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7657.15</v>
+        <v>7358.74</v>
       </c>
       <c r="C7" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -745,13 +745,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>140167</v>
+        <v>151315</v>
       </c>
       <c r="H7" t="n">
-        <v>62.06</v>
+        <v>69.36</v>
       </c>
       <c r="I7" t="n">
-        <v>3.452</v>
+        <v>3.29</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -769,10 +769,10 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>182.3509895</v>
+        <v>214.7027646</v>
       </c>
       <c r="P7" t="n">
-        <v>7.866000000000001</v>
+        <v>7.143</v>
       </c>
       <c r="Q7" t="n">
         <v>6</v>
@@ -785,13 +785,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20265.01</v>
+        <v>21254.705</v>
       </c>
       <c r="C8" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -800,34 +800,34 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>202505</v>
+        <v>202307</v>
       </c>
       <c r="H8" t="n">
-        <v>74.25</v>
+        <v>80.84</v>
       </c>
       <c r="I8" t="n">
-        <v>3.735</v>
+        <v>3.594</v>
       </c>
       <c r="J8" t="n">
-        <v>2753.9</v>
+        <v>2797.26</v>
       </c>
       <c r="K8" t="n">
-        <v>2.63</v>
+        <v>7.64</v>
       </c>
       <c r="L8" t="n">
-        <v>4.36</v>
+        <v>4.54</v>
       </c>
       <c r="M8" t="n">
-        <v>415.36</v>
+        <v>536.8200000000001</v>
       </c>
       <c r="N8" t="n">
-        <v>2146.94</v>
+        <v>2093.48</v>
       </c>
       <c r="O8" t="n">
-        <v>212.412888</v>
+        <v>219.8118854</v>
       </c>
       <c r="P8" t="n">
-        <v>8.567</v>
+        <v>7.808</v>
       </c>
       <c r="Q8" t="n">
         <v>9</v>
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>693099.36</v>
+        <v>385051.04</v>
       </c>
       <c r="C9" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
         <v>99</v>
@@ -852,37 +852,37 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>219622</v>
+        <v>205863</v>
       </c>
       <c r="H9" t="n">
-        <v>100.14</v>
+        <v>93.34</v>
       </c>
       <c r="I9" t="n">
-        <v>4.468</v>
+        <v>3.907</v>
       </c>
       <c r="J9" t="n">
-        <v>88646.75999999999</v>
+        <v>75149.78999999999</v>
       </c>
       <c r="K9" t="n">
-        <v>104519.54</v>
+        <v>92523.94</v>
       </c>
       <c r="L9" t="n">
-        <v>141630.61</v>
+        <v>83340.33</v>
       </c>
       <c r="M9" t="n">
-        <v>67474.85000000001</v>
+        <v>48159.86</v>
       </c>
       <c r="N9" t="n">
-        <v>108519.28</v>
+        <v>36430.33</v>
       </c>
       <c r="O9" t="n">
-        <v>227.2328068</v>
+        <v>226.9873637</v>
       </c>
       <c r="P9" t="n">
-        <v>14.313</v>
+        <v>8.622999999999999</v>
       </c>
       <c r="Q9" t="n">
         <v>12</v>

</xml_diff>